<commit_message>
finished scraped CSV: vivino_wine_final.csv
</commit_message>
<xml_diff>
--- a/URLs.xlsx
+++ b/URLs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeongwooHan\Desktop\Project_WebScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73503D52-2B04-4922-BD65-A83F6B148230}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4759229C-CAE2-4314-8BB3-61D7283FCBEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2D8B3C70-3BD6-430D-AF82-3ABF7E1FC4FE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Start</t>
   </si>
@@ -81,9 +81,6 @@
     <t>https://www.vivino.com/explore?e=eJzLLbI1VMvNzLM1tFDLTaywNbRUS660DQ1WSwYSLmoFQNn0NNuyxKLM1JLEHLX8JFu1fFu18pLoWKBMsW1JBQCYExSV</t>
   </si>
   <si>
-    <t>https://www.vivino.com/explore?e=eJzLLbI1VMvNzLM1tFTLTaywNTJQS660DQ1WSwYSLmoFQNn0NNuyxKLM1JLEHLX8JFu1fFu18pLoWKBMsW1JBQCWyxSO</t>
-  </si>
-  <si>
     <t>https://www.vivino.com/explore?e=eJzLLbI1VMvNzLM1MlDLTaywNTJUS660DQ1WSwYSLmoFQNn0NNuyxKLM1JLEHLX8JFu1fFu18pLoWKBMsW1JBQCVRBSH</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>https://www.vivino.com/explore?e=eJw1yjsOgDAMA9DbeIYJlmzcADEhhhBaVIkCasvv9nRoFvtJtg9Uw7udmgqeX2oryEdDD8nR4czraunm4EziDcdMOAhPGqe8yBdzc1BcilQgW4HVz2IKTv2YiEjCPxGELmM%3D</t>
+  </si>
+  <si>
+    <t>https://www.vivino.com/explore?e=eJzLLbI11jNVy83MszW0VMtNrLA1MlBLrrQNDVZLBhIuagW2hmrpabZliUWZqSWJOWr5SbZq-bZq5SXRsUCZ5MpiIJ1ZAmWUFqsV2yYnAgBpRxtk</t>
+  </si>
+  <si>
+    <t>https://www.vivino.com/explore?e=eJzLLbI11jNVy83MszW0VMtNrLA1MlBLrrQNDVZLBhIuagW2hmrpabZliUWZqSWJOWr5SbZq-bZq5SXRsUCZ5MpiIJ1YBGOUwhglUEZyDpSRBlOTkgplFMDUpBarFdsmJwIAR9EuxQ%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -543,11 +546,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D768CA-35A8-4920-B3D6-C6E1A58B2407}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -727,192 +728,192 @@
         <v>20</v>
       </c>
       <c r="C13">
-        <v>1373</v>
+        <v>966</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>19</v>
+      </c>
+      <c r="B14">
         <v>20</v>
       </c>
-      <c r="B14">
-        <v>21</v>
-      </c>
       <c r="C14">
-        <v>643</v>
+        <v>857</v>
       </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15">
         <v>21</v>
       </c>
-      <c r="B15">
-        <v>22</v>
-      </c>
       <c r="C15">
-        <v>706</v>
+        <v>643</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>21</v>
+      </c>
+      <c r="B16">
         <v>22</v>
       </c>
-      <c r="B16">
-        <v>23</v>
-      </c>
       <c r="C16">
-        <v>610</v>
+        <v>706</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="B17">
         <v>23</v>
       </c>
-      <c r="B17">
-        <v>24</v>
-      </c>
       <c r="C17">
-        <v>534</v>
+        <v>610</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>23</v>
+      </c>
+      <c r="B18">
         <v>24</v>
       </c>
-      <c r="B18">
-        <v>25</v>
-      </c>
       <c r="C18">
-        <v>948</v>
+        <v>534</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>24</v>
+      </c>
+      <c r="B19">
         <v>25</v>
       </c>
-      <c r="B19">
-        <v>27</v>
-      </c>
       <c r="C19">
-        <v>888</v>
+        <v>948</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>25</v>
+      </c>
+      <c r="B20">
         <v>27</v>
       </c>
-      <c r="B20">
-        <v>29</v>
-      </c>
       <c r="C20">
-        <v>944</v>
+        <v>888</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>27</v>
+      </c>
+      <c r="B21">
         <v>29</v>
       </c>
-      <c r="B21">
-        <v>30</v>
-      </c>
       <c r="C21">
-        <v>988</v>
+        <v>944</v>
       </c>
       <c r="D21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22">
         <v>30</v>
       </c>
-      <c r="B22">
-        <v>33</v>
-      </c>
       <c r="C22">
-        <v>1001</v>
+        <v>988</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23">
         <v>33</v>
       </c>
-      <c r="B23">
-        <v>35</v>
-      </c>
       <c r="C23">
-        <v>986</v>
+        <v>1001</v>
       </c>
       <c r="D23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>33</v>
+      </c>
+      <c r="B24">
         <v>35</v>
       </c>
-      <c r="B24">
-        <v>38</v>
-      </c>
       <c r="C24">
-        <v>1053</v>
+        <v>986</v>
       </c>
       <c r="D24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>35</v>
+      </c>
+      <c r="B25">
         <v>38</v>
       </c>
-      <c r="B25">
-        <v>40</v>
-      </c>
       <c r="C25">
-        <v>1102</v>
+        <v>1053</v>
       </c>
       <c r="D25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>38</v>
+      </c>
+      <c r="B26">
         <v>40</v>
       </c>
-      <c r="B26">
-        <v>45</v>
-      </c>
       <c r="C26">
-        <v>1160</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>38</v>
+        <v>1102</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -923,24 +924,24 @@
         <v>45</v>
       </c>
       <c r="C27">
-        <v>933</v>
+        <v>1160</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28">
         <v>45</v>
       </c>
-      <c r="B28">
-        <v>50</v>
-      </c>
       <c r="C28">
-        <v>1300</v>
+        <v>933</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -951,24 +952,24 @@
         <v>50</v>
       </c>
       <c r="C29">
-        <v>972</v>
-      </c>
-      <c r="D29" t="s">
-        <v>41</v>
+        <v>1300</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>45</v>
+      </c>
+      <c r="B30">
         <v>50</v>
       </c>
-      <c r="B30">
-        <v>60</v>
-      </c>
       <c r="C30">
-        <v>1126</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>42</v>
+        <v>972</v>
+      </c>
+      <c r="D30" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -979,10 +980,10 @@
         <v>60</v>
       </c>
       <c r="C31">
-        <v>1037</v>
+        <v>1126</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -993,24 +994,24 @@
         <v>60</v>
       </c>
       <c r="C32">
-        <v>1190</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
+        <v>1037</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>50</v>
+      </c>
+      <c r="B33">
         <v>60</v>
       </c>
-      <c r="B33">
-        <v>70</v>
-      </c>
       <c r="C33">
-        <v>1479</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>45</v>
+        <v>1190</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1021,24 +1022,24 @@
         <v>70</v>
       </c>
       <c r="C34">
-        <v>1026</v>
-      </c>
-      <c r="D34" t="s">
-        <v>46</v>
+        <v>1479</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
+        <v>60</v>
+      </c>
+      <c r="B35">
         <v>70</v>
       </c>
-      <c r="B35">
-        <v>80</v>
-      </c>
       <c r="C35">
-        <v>1212</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>47</v>
+        <v>1026</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1049,150 +1050,164 @@
         <v>80</v>
       </c>
       <c r="C36">
-        <v>937</v>
+        <v>1212</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
+        <v>70</v>
+      </c>
+      <c r="B37">
         <v>80</v>
       </c>
-      <c r="B37">
-        <v>90</v>
-      </c>
       <c r="C37">
-        <v>1245</v>
+        <v>937</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
+        <v>80</v>
+      </c>
+      <c r="B38">
         <v>90</v>
       </c>
-      <c r="B38">
-        <v>100</v>
-      </c>
       <c r="C38">
-        <v>1259</v>
+        <v>1245</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
+        <v>90</v>
+      </c>
+      <c r="B39">
         <v>100</v>
       </c>
-      <c r="B39">
-        <v>110</v>
-      </c>
       <c r="C39">
-        <v>771</v>
+        <v>1259</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
+        <v>100</v>
+      </c>
+      <c r="B40">
         <v>110</v>
       </c>
-      <c r="B40">
-        <v>120</v>
-      </c>
       <c r="C40">
-        <v>730</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
+        <v>771</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>110</v>
+      </c>
+      <c r="B41">
         <v>120</v>
       </c>
-      <c r="B41">
-        <v>140</v>
-      </c>
       <c r="C41">
-        <v>1087</v>
+        <v>730</v>
       </c>
       <c r="D41" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>120</v>
+      </c>
+      <c r="B42">
         <v>140</v>
       </c>
-      <c r="B42">
-        <v>170</v>
-      </c>
       <c r="C42">
-        <v>1166</v>
+        <v>1087</v>
       </c>
       <c r="D42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43">
+        <v>140</v>
+      </c>
+      <c r="B43">
         <v>170</v>
       </c>
-      <c r="B43">
-        <v>200</v>
-      </c>
       <c r="C43">
-        <v>971</v>
+        <v>1166</v>
       </c>
       <c r="D43" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>170</v>
+      </c>
+      <c r="B44">
         <v>200</v>
       </c>
-      <c r="B44">
-        <v>250</v>
-      </c>
       <c r="C44">
-        <v>841</v>
+        <v>971</v>
       </c>
       <c r="D44" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>200</v>
+      </c>
+      <c r="B45">
         <v>250</v>
       </c>
-      <c r="B45">
-        <v>350</v>
-      </c>
       <c r="C45">
-        <v>1023</v>
+        <v>841</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>250</v>
+      </c>
+      <c r="B46">
         <v>350</v>
       </c>
-      <c r="B46">
+      <c r="C46">
+        <v>1023</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>350</v>
+      </c>
+      <c r="B47">
         <v>450</v>
       </c>
-      <c r="C46">
+      <c r="C47">
         <v>615</v>
       </c>
-      <c r="D46" t="s">
-        <v>37</v>
+      <c r="D47" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1201,14 +1216,15 @@
     <hyperlink ref="D9" r:id="rId2" xr:uid="{25BD99F9-D8EE-49F9-9254-1399AFB5DE8E}"/>
     <hyperlink ref="D10" r:id="rId3" xr:uid="{20624D04-6DE8-4995-AFD3-FD89BB7618FB}"/>
     <hyperlink ref="D12" r:id="rId4" xr:uid="{81A6DD84-4347-44FA-8C78-D7CF83A14551}"/>
-    <hyperlink ref="D26" r:id="rId5" xr:uid="{9110702B-504D-4C56-A03F-FBB0BD42D75C}"/>
-    <hyperlink ref="D28" r:id="rId6" xr:uid="{A9F9D89C-1B2D-437C-9B01-F30593032CBD}"/>
-    <hyperlink ref="D33" r:id="rId7" xr:uid="{EFD85B8D-2AB8-442E-8B73-A235FE43219B}"/>
-    <hyperlink ref="D35" r:id="rId8" xr:uid="{26036DC9-90EE-49ED-8983-26071D28DA8F}"/>
-    <hyperlink ref="D37" r:id="rId9" xr:uid="{5CAC734E-6579-46E8-BCD7-4292BF81490F}"/>
-    <hyperlink ref="D38" r:id="rId10" xr:uid="{C7E8232E-BAAE-4738-AAB9-94DC31642DE6}"/>
-    <hyperlink ref="D39" r:id="rId11" xr:uid="{A417F585-BA10-4A61-8B3F-555B1ACE5CE4}"/>
-    <hyperlink ref="D36" r:id="rId12" xr:uid="{B5BE1BF9-BE6A-47B6-82B0-8115142EE137}"/>
+    <hyperlink ref="D27" r:id="rId5" xr:uid="{9110702B-504D-4C56-A03F-FBB0BD42D75C}"/>
+    <hyperlink ref="D29" r:id="rId6" xr:uid="{A9F9D89C-1B2D-437C-9B01-F30593032CBD}"/>
+    <hyperlink ref="D34" r:id="rId7" xr:uid="{EFD85B8D-2AB8-442E-8B73-A235FE43219B}"/>
+    <hyperlink ref="D36" r:id="rId8" xr:uid="{26036DC9-90EE-49ED-8983-26071D28DA8F}"/>
+    <hyperlink ref="D38" r:id="rId9" xr:uid="{5CAC734E-6579-46E8-BCD7-4292BF81490F}"/>
+    <hyperlink ref="D39" r:id="rId10" xr:uid="{C7E8232E-BAAE-4738-AAB9-94DC31642DE6}"/>
+    <hyperlink ref="D40" r:id="rId11" xr:uid="{A417F585-BA10-4A61-8B3F-555B1ACE5CE4}"/>
+    <hyperlink ref="D37" r:id="rId12" xr:uid="{B5BE1BF9-BE6A-47B6-82B0-8115142EE137}"/>
+    <hyperlink ref="C14" r:id="rId13" display="https://www.vivino.com/explore?e=eJzLLbI11jNVy83MszW0VMtNrLA1MlBLrrQNDVZLBhIuagW2hmrpabZliUWZqSWJOWr5SbZq-bZq5SXRsUCZ5MpiIJ1ZAmWUFqsV2yYnAgBpRxtk" xr:uid="{FE81AED3-52D6-48A5-B280-7DA98D1E7CF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>